<commit_message>
Analyse du problème logistique et traduction
</commit_message>
<xml_diff>
--- a/26. Recherche opérationnelle en Excel/06 - TRANSPORT - OPTIMISATION LOGISTIQUE INTERNATIONALE/Programme linéaire traduit et analyse.xlsx
+++ b/26. Recherche opérationnelle en Excel/06 - TRANSPORT - OPTIMISATION LOGISTIQUE INTERNATIONALE/Programme linéaire traduit et analyse.xlsx
@@ -65,10 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
-  <si>
-    <t>Supply Region</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
   <si>
     <t>N. America</t>
   </si>
@@ -97,27 +94,9 @@
     <t>(1=open)</t>
   </si>
   <si>
-    <t>Constraints</t>
-  </si>
-  <si>
-    <t>Excess Capacity</t>
-  </si>
-  <si>
-    <t>Unmet Demand</t>
-  </si>
-  <si>
-    <t>Objective Function</t>
-  </si>
-  <si>
-    <t>Cost =</t>
-  </si>
-  <si>
     <t>Région fournisseur</t>
   </si>
   <si>
-    <t>Demande</t>
-  </si>
-  <si>
     <t>Coût ($)</t>
   </si>
   <si>
@@ -136,9 +115,6 @@
     <t>Grandes usines</t>
   </si>
   <si>
-    <t xml:space="preserve">Fixe </t>
-  </si>
-  <si>
     <t>Bas</t>
   </si>
   <si>
@@ -154,8 +130,32 @@
     <t>Usines</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Coût de production et transport pour 1,000,000 Unités</t>
+    <t>Capacité excédentaire</t>
+  </si>
+  <si>
+    <t>Contraintes</t>
+  </si>
+  <si>
+    <t>Demande non satisfaite</t>
+  </si>
+  <si>
+    <t>Fonction objectif</t>
+  </si>
+  <si>
+    <t>Coût =</t>
+  </si>
+  <si>
+    <t>Région fournisseuse</t>
+  </si>
+  <si>
+    <t>Région qui demande
+Coût de production et transport pour 1,000,000 Unités (en millions $ )</t>
+  </si>
+  <si>
+    <t>Demande(en millions d'unités)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coût Fixe </t>
   </si>
 </sst>
 </file>
@@ -214,7 +214,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,8 +239,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="36">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -576,19 +582,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -675,20 +668,7 @@
   </cellStyleXfs>
   <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -714,7 +694,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
@@ -751,16 +730,14 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -770,7 +747,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -809,10 +786,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -825,7 +799,26 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -849,10 +842,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>558165</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>367665</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>32385</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4539448" cy="1470146"/>
     <xdr:sp macro="" textlink="">
@@ -868,7 +861,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7225665" y="6029325"/>
+          <a:off x="2272665" y="6638925"/>
           <a:ext cx="4539448" cy="1470146"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -978,9 +971,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>121920</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -990,7 +983,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7261860" y="1021080"/>
-          <a:ext cx="5013960" cy="960120"/>
+          <a:ext cx="5158740" cy="1272540"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1028,6 +1021,12 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
+            <a:rPr lang="fr-FR" b="1"/>
+            <a:t>L'histoire : </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
             <a:rPr lang="fr-FR"/>
             <a:t>Le vice-président de la chaîne d'approvisionnement de SunOil réfléchit à l'endroit où construire de nouvelles installations de production. Il y a cinq options : Amérique du Nord et du Sud, Europe, Asie et Afrique. le total, les coûts de production et de transport pour chaque couple possible de régions « Offre » et « Demande » sont indiqués dans le tableau à gauche</a:t>
           </a:r>
@@ -1039,16 +1038,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>594360</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1057,7 +1056,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7261860" y="1988820"/>
+          <a:off x="7284720" y="2522220"/>
           <a:ext cx="5166360" cy="3771900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1097,7 +1096,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="fr-FR"/>
-            <a:t>Par exemple, il en coûte 115 000 $ pour produire 1 million d'unités en Asie et les transporter en Amérique du Nord. Pour simplifier, nous supposons que ces coûts sont constants et que chaque million d'unités nous coûte la même chose à produire et à transporter. De plus, la construction d'une usine a un coût fixe qui ne dépend pas du volume de production. Il existe deux types d'usines possibles : une faible capacité qui peut produire jusqu'à 10 millions d'unités par an à un coût fixe qui dépend de la région et est donné dans les cellules G4:G8 de la Fig. 1, et une grande capacité qui peut produire jusqu'à 20 millions d'unités. millions d'unités par an à un coût fixe supérieur de 50 % (présentant ainsi des économies d'échelle). Le coût associé et la capacité maximale sont indiqués dans les cellules I4:J8 de la Figure 5.</a:t>
+            <a:t>Par exemple, il en coûte 115 000 $ pour produire 1 million d'unités en Asie et les transporter en Amérique du Nord(B7). Pour simplifier, nous supposons que ces coûts sont constants et que chaque million d'unités nous coûte la même chose à produire et à transporter. De plus, la construction d'une usine a un coût fixe qui ne dépend pas du volume de production. Il existe deux types d'usines possibles : une faible capacité qui peut produire jusqu'à 10 millions d'unités par an à un coût fixe qui dépend de la région et est donné dans les cellules G4:G8 de la Fig. 1, et une grande capacité qui peut produire jusqu'à 20 millions d'unités. millions d'unités par an à un coût fixe supérieur de 50 % (présentant ainsi des économies d'échelle). Le coût associé et la capacité maximale sont indiqués dans les cellules I4:J8 de la Figure 5.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1403,657 +1402,662 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="1" max="1" width="26.21875" customWidth="1"/>
     <col min="2" max="3" width="10" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" customWidth="1"/>
-    <col min="9" max="9" width="7.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="75" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+    </row>
+    <row r="2" spans="1:21" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="B2" s="68" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="79" t="s">
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="83" t="s">
+      <c r="H2" s="81" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="82" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="83" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="67" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="67"/>
+      <c r="P2" s="67"/>
+      <c r="Q2" s="67"/>
+      <c r="R2" s="67"/>
+      <c r="S2" s="67"/>
+      <c r="T2" s="67"/>
+      <c r="U2" s="67"/>
+    </row>
+    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="83"/>
-      <c r="N2" s="83"/>
-      <c r="O2" s="83"/>
-      <c r="P2" s="83"/>
-      <c r="Q2" s="83"/>
-      <c r="R2" s="83"/>
-      <c r="S2" s="83"/>
-      <c r="T2" s="83"/>
-      <c r="U2" s="83"/>
-    </row>
-    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="76"/>
-      <c r="M3" s="77"/>
-      <c r="N3" s="77"/>
-      <c r="O3" s="77"/>
-      <c r="P3" s="77"/>
-      <c r="Q3" s="77"/>
-      <c r="R3" s="77"/>
-      <c r="S3" s="77"/>
-      <c r="T3" s="78"/>
+      <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="72"/>
+      <c r="M3" s="73"/>
+      <c r="N3" s="73"/>
+      <c r="O3" s="73"/>
+      <c r="P3" s="73"/>
+      <c r="Q3" s="73"/>
+      <c r="R3" s="73"/>
+      <c r="S3" s="73"/>
+      <c r="T3" s="73"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="63">
+      <c r="A4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="55">
         <v>81</v>
       </c>
-      <c r="C4" s="64">
+      <c r="C4" s="56">
         <v>92</v>
       </c>
-      <c r="D4" s="64">
+      <c r="D4" s="56">
         <v>101</v>
       </c>
-      <c r="E4" s="64">
+      <c r="E4" s="56">
         <v>130</v>
       </c>
-      <c r="F4" s="65">
+      <c r="F4" s="57">
         <v>115</v>
       </c>
-      <c r="G4" s="66">
+      <c r="G4" s="58">
         <v>6000</v>
       </c>
-      <c r="H4" s="67">
+      <c r="H4" s="59">
         <v>10</v>
       </c>
-      <c r="I4" s="68">
+      <c r="I4" s="60">
         <f>1.5*G4</f>
         <v>9000</v>
       </c>
-      <c r="J4" s="69">
+      <c r="J4" s="61">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="63">
+      <c r="A5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="55">
         <v>117</v>
       </c>
-      <c r="C5" s="64">
+      <c r="C5" s="56">
         <v>77</v>
       </c>
-      <c r="D5" s="64">
+      <c r="D5" s="56">
         <v>108</v>
       </c>
-      <c r="E5" s="64">
+      <c r="E5" s="56">
         <v>98</v>
       </c>
-      <c r="F5" s="65">
+      <c r="F5" s="57">
         <v>100</v>
       </c>
-      <c r="G5" s="66">
+      <c r="G5" s="58">
         <v>4500</v>
       </c>
-      <c r="H5" s="67">
+      <c r="H5" s="59">
         <v>10</v>
       </c>
-      <c r="I5" s="68">
+      <c r="I5" s="60">
         <f>1.5*G5</f>
         <v>6750</v>
       </c>
-      <c r="J5" s="69">
+      <c r="J5" s="61">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="63">
+      <c r="A6" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="55">
         <v>102</v>
       </c>
-      <c r="C6" s="64">
+      <c r="C6" s="56">
         <v>105</v>
       </c>
-      <c r="D6" s="64">
+      <c r="D6" s="56">
         <v>95</v>
       </c>
-      <c r="E6" s="64">
+      <c r="E6" s="56">
         <v>119</v>
       </c>
-      <c r="F6" s="65">
+      <c r="F6" s="57">
         <v>111</v>
       </c>
-      <c r="G6" s="66">
+      <c r="G6" s="58">
         <v>6500</v>
       </c>
-      <c r="H6" s="67">
+      <c r="H6" s="59">
         <v>10</v>
       </c>
-      <c r="I6" s="68">
+      <c r="I6" s="60">
         <f>1.5*G6</f>
         <v>9750</v>
       </c>
-      <c r="J6" s="69">
+      <c r="J6" s="61">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="63">
+      <c r="A7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="55">
         <v>115</v>
       </c>
-      <c r="C7" s="64">
+      <c r="C7" s="56">
         <v>125</v>
       </c>
-      <c r="D7" s="64">
+      <c r="D7" s="56">
         <v>90</v>
       </c>
-      <c r="E7" s="64">
+      <c r="E7" s="56">
         <v>59</v>
       </c>
-      <c r="F7" s="65">
+      <c r="F7" s="57">
         <v>74</v>
       </c>
-      <c r="G7" s="66">
+      <c r="G7" s="58">
         <v>4100</v>
       </c>
-      <c r="H7" s="67">
+      <c r="H7" s="59">
         <v>10</v>
       </c>
-      <c r="I7" s="68">
+      <c r="I7" s="60">
         <f>1.5*G7</f>
         <v>6150</v>
       </c>
-      <c r="J7" s="69">
+      <c r="J7" s="61">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="70">
+      <c r="A8" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="62">
         <v>142</v>
       </c>
-      <c r="C8" s="71">
+      <c r="C8" s="63">
         <v>100</v>
       </c>
-      <c r="D8" s="71">
+      <c r="D8" s="63">
         <v>103</v>
       </c>
-      <c r="E8" s="71">
+      <c r="E8" s="63">
         <v>105</v>
       </c>
-      <c r="F8" s="72">
+      <c r="F8" s="64">
         <v>71</v>
       </c>
-      <c r="G8" s="66">
+      <c r="G8" s="58">
         <v>4000</v>
       </c>
-      <c r="H8" s="67">
+      <c r="H8" s="59">
         <v>10</v>
       </c>
-      <c r="I8" s="68">
+      <c r="I8" s="60">
         <f>1.5*G8</f>
         <v>6000</v>
       </c>
-      <c r="J8" s="69">
+      <c r="J8" s="61">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="12">
+        <v>12</v>
+      </c>
+      <c r="C9" s="13">
+        <v>8</v>
+      </c>
+      <c r="D9" s="13">
+        <v>14</v>
+      </c>
+      <c r="E9" s="13">
         <v>16</v>
       </c>
-      <c r="B9" s="17">
-        <v>12</v>
-      </c>
-      <c r="C9" s="18">
+      <c r="F9" s="14">
+        <v>7</v>
+      </c>
+      <c r="G9" s="15"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="17"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10" s="18"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+    </row>
+    <row r="11" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="77" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="78"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+    </row>
+    <row r="12" spans="1:21" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1"/>
+      <c r="B12" s="70" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="71"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="65" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="66" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="L12" s="74"/>
+      <c r="M12" s="74"/>
+      <c r="N12" s="74"/>
+      <c r="O12" s="74"/>
+      <c r="P12" s="74"/>
+      <c r="Q12" s="74"/>
+      <c r="R12" s="74"/>
+    </row>
+    <row r="13" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="18">
-        <v>14</v>
-      </c>
-      <c r="E9" s="18">
-        <v>16</v>
-      </c>
-      <c r="F9" s="19">
-        <v>7</v>
-      </c>
-      <c r="G9" s="20"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="22"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="23"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-    </row>
-    <row r="11" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-    </row>
-    <row r="12" spans="1:21" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-      <c r="B12" s="81" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="82"/>
-      <c r="D12" s="82"/>
-      <c r="E12" s="82"/>
-      <c r="F12" s="82"/>
-      <c r="G12" s="73" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" s="74" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" s="25" t="s">
+      <c r="H13" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="L12" s="75"/>
-      <c r="M12" s="75"/>
-      <c r="N12" s="75"/>
-      <c r="O12" s="75"/>
-      <c r="P12" s="75"/>
-      <c r="Q12" s="75"/>
-      <c r="R12" s="75"/>
-    </row>
-    <row r="13" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="27" t="s">
+      <c r="I13" s="24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="25">
+        <v>0</v>
+      </c>
+      <c r="C14" s="26">
+        <v>0</v>
+      </c>
+      <c r="D14" s="26">
+        <v>0</v>
+      </c>
+      <c r="E14" s="26">
+        <v>1.5100933910272563E-7</v>
+      </c>
+      <c r="F14" s="27">
+        <v>0</v>
+      </c>
+      <c r="G14" s="28">
+        <v>0</v>
+      </c>
+      <c r="H14" s="29">
+        <v>0</v>
+      </c>
+      <c r="I14" s="30">
+        <f>G14+H14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="G13" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="I13" s="30" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
+      <c r="B15" s="25">
+        <v>11.99999998491036</v>
+      </c>
+      <c r="C15" s="26">
+        <v>8.0000000129577327</v>
+      </c>
+      <c r="D15" s="26">
+        <v>0</v>
+      </c>
+      <c r="E15" s="31">
+        <v>0</v>
+      </c>
+      <c r="F15" s="32">
+        <v>0</v>
+      </c>
+      <c r="G15" s="33">
+        <v>0</v>
+      </c>
+      <c r="H15" s="34">
         <v>1</v>
       </c>
-      <c r="B14" s="31">
-        <v>0</v>
-      </c>
-      <c r="C14" s="32">
-        <v>0</v>
-      </c>
-      <c r="D14" s="32">
-        <v>0</v>
-      </c>
-      <c r="E14" s="32">
-        <v>1.5100933910272563E-7</v>
-      </c>
-      <c r="F14" s="33">
-        <v>0</v>
-      </c>
-      <c r="G14" s="34">
-        <v>0</v>
-      </c>
-      <c r="H14" s="35">
-        <v>0</v>
-      </c>
-      <c r="I14" s="36">
-        <f>G14+H14</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="31">
-        <v>11.99999998491036</v>
-      </c>
-      <c r="C15" s="32">
-        <v>8.0000000129577327</v>
-      </c>
-      <c r="D15" s="32">
-        <v>0</v>
-      </c>
-      <c r="E15" s="37">
-        <v>0</v>
-      </c>
-      <c r="F15" s="38">
-        <v>0</v>
-      </c>
-      <c r="G15" s="39">
-        <v>0</v>
-      </c>
-      <c r="H15" s="40">
-        <v>1</v>
-      </c>
-      <c r="I15" s="36">
+      <c r="I15" s="30">
         <f>G15+H15</f>
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="25">
+        <v>0</v>
+      </c>
+      <c r="C16" s="26">
+        <v>0</v>
+      </c>
+      <c r="D16" s="26">
+        <v>0</v>
+      </c>
+      <c r="E16" s="31">
+        <v>0</v>
+      </c>
+      <c r="F16" s="32">
+        <v>0</v>
+      </c>
+      <c r="G16" s="33">
+        <v>0</v>
+      </c>
+      <c r="H16" s="34">
+        <v>0</v>
+      </c>
+      <c r="I16" s="30">
+        <f>G16+H16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="31">
-        <v>0</v>
-      </c>
-      <c r="C16" s="32">
-        <v>0</v>
-      </c>
-      <c r="D16" s="32">
-        <v>0</v>
-      </c>
-      <c r="E16" s="37">
-        <v>0</v>
-      </c>
-      <c r="F16" s="38">
-        <v>0</v>
-      </c>
-      <c r="G16" s="39">
-        <v>0</v>
-      </c>
-      <c r="H16" s="40">
-        <v>0</v>
-      </c>
-      <c r="I16" s="36">
-        <f>G16+H16</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="31">
-        <v>0</v>
-      </c>
-      <c r="C17" s="32">
-        <v>0</v>
-      </c>
-      <c r="D17" s="32">
+      <c r="B17" s="25">
+        <v>0</v>
+      </c>
+      <c r="C17" s="26">
+        <v>0</v>
+      </c>
+      <c r="D17" s="26">
         <v>4.0000001510097185</v>
       </c>
-      <c r="E17" s="32">
+      <c r="E17" s="26">
         <v>15.99999984899028</v>
       </c>
-      <c r="F17" s="33">
-        <v>0</v>
-      </c>
-      <c r="G17" s="34">
-        <v>0</v>
-      </c>
-      <c r="H17" s="35">
+      <c r="F17" s="27">
+        <v>0</v>
+      </c>
+      <c r="G17" s="28">
+        <v>0</v>
+      </c>
+      <c r="H17" s="29">
         <v>1</v>
       </c>
-      <c r="I17" s="36">
+      <c r="I17" s="30">
         <f>G17+H17</f>
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="42">
-        <v>0</v>
-      </c>
-      <c r="C18" s="43">
-        <v>0</v>
-      </c>
-      <c r="D18" s="43">
+      <c r="A18" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="36">
+        <v>0</v>
+      </c>
+      <c r="C18" s="37">
+        <v>0</v>
+      </c>
+      <c r="D18" s="37">
         <v>10.000000333764245</v>
       </c>
-      <c r="E18" s="43">
-        <v>0</v>
-      </c>
-      <c r="F18" s="44">
+      <c r="E18" s="37">
+        <v>0</v>
+      </c>
+      <c r="F18" s="38">
         <v>6.9999999999999991</v>
       </c>
-      <c r="G18" s="45">
-        <v>0</v>
-      </c>
-      <c r="H18" s="29">
+      <c r="G18" s="39">
+        <v>0</v>
+      </c>
+      <c r="H18" s="23">
         <v>1</v>
       </c>
-      <c r="I18" s="46">
+      <c r="I18" s="40">
         <f>G18+H18</f>
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
+      <c r="A20" s="79" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="76"/>
+      <c r="C20" s="76"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+    </row>
+    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="53">
+      <c r="A22" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="45">
         <f>G14*H4+H14*J4-SUM(B14:F14)</f>
         <v>-1.5100933910272563E-7</v>
       </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" s="31">
+      <c r="A23" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="25">
         <f>G15*H5+H15*J5-SUM(B15:F15)</f>
         <v>2.131905318947247E-9</v>
       </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="25">
+        <f>G16*H6+H16*J6-SUM(B16:F16)</f>
+        <v>0</v>
+      </c>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="31">
-        <f>G16*H6+H16*J6-SUM(B16:F16)</f>
-        <v>0</v>
-      </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="14" t="s">
+      <c r="B25" s="25">
+        <f>G17*H7+H17*J7-SUM(B17:F17)</f>
+        <v>0</v>
+      </c>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+    </row>
+    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="31">
-        <f>G17*H7+H17*J7-SUM(B17:F17)</f>
-        <v>0</v>
-      </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-    </row>
-    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="42">
+      <c r="B26" s="36">
         <f>G18*H8+H18*J8-SUM(B18:F18)</f>
         <v>2.9999996662357553</v>
       </c>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="54"/>
-      <c r="B27" s="55" t="s">
+      <c r="A27" s="46"/>
+      <c r="B27" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="55" t="s">
+      <c r="D27" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="55" t="s">
+      <c r="E27" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="55" t="s">
+      <c r="F27" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F27" s="56" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="60">
+      <c r="A28" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="52">
         <f>B9-SUM(B14:B18)</f>
         <v>1.508963975993538E-8</v>
       </c>
-      <c r="C28" s="61">
+      <c r="C28" s="53">
         <f>C9-SUM(C14:C18)</f>
         <v>-1.2957732664631294E-8</v>
       </c>
-      <c r="D28" s="61">
+      <c r="D28" s="53">
         <f>D9-SUM(D14:D18)</f>
         <v>-4.8477396319412946E-7</v>
       </c>
-      <c r="E28" s="61">
+      <c r="E28" s="53">
         <f>E9-SUM(E14:E18)</f>
         <v>3.8191672047105385E-13</v>
       </c>
-      <c r="F28" s="62">
+      <c r="F28" s="54">
         <f>F9-SUM(F14:F18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A30" s="75" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="76"/>
+      <c r="C30" s="76"/>
     </row>
     <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="57" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31" s="58">
+      <c r="A31" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="50">
         <f>SUMPRODUCT(B14:F18,B4:F8)+SUMPRODUCT(G14:G18,G4:G8)+SUMPRODUCT(H14:H18,I4:I8)</f>
         <v>23751.000057922491</v>
       </c>
-      <c r="D31" s="59"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>